<commit_message>
add last day plots
</commit_message>
<xml_diff>
--- a/RawData/元宝血糖记录.xlsx
+++ b/RawData/元宝血糖记录.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>日期 dd-mm-yyyy</t>
   </si>
@@ -27,7 +27,7 @@
     <t>血糖  /  mmol/L</t>
   </si>
   <si>
-    <t>胰岛素 / μl</t>
+    <t>胰岛素 / unit</t>
   </si>
   <si>
     <t>备注</t>
@@ -85,16 +85,26 @@
   </si>
   <si>
     <t>罐头12g</t>
+  </si>
+  <si>
+    <t>16-09-2020</t>
+  </si>
+  <si>
+    <t>猫粮3g</t>
+  </si>
+  <si>
+    <t>鸡胸35g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
     <numFmt numFmtId="165" formatCode="yyyy/m/d h:mm:ss;@"/>
     <numFmt numFmtId="166" formatCode="yyyy/m/d"/>
+    <numFmt numFmtId="167" formatCode="h:mm:ss;@"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -132,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyBorder="true" quotePrefix="false" applyNumberFormat="false" applyFont="true">
       <alignment vertical="center" wrapText="false"/>
@@ -167,6 +177,9 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyBorder="true" quotePrefix="false" applyNumberFormat="true" applyFont="true">
       <alignment vertical="center" wrapText="false"/>
     </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyBorder="true" quotePrefix="false" applyNumberFormat="true" applyFont="true">
+      <alignment vertical="center" wrapText="false"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -942,53 +955,200 @@
       </c>
     </row>
     <row r="85">
-</row>
+      <c r="B85" s="4" t="n">
+        <v>0.8652777777777778</v>
+      </c>
+      <c r="D85" s="6" t="n">
+        <v>3.9</v>
+      </c>
+    </row>
     <row r="86">
-</row>
+      <c r="B86" s="4" t="n">
+        <v>0.8993055555555556</v>
+      </c>
+      <c r="D86" s="6" t="n">
+        <v>5.3</v>
+      </c>
+    </row>
     <row r="87">
-</row>
+      <c r="B87" s="4" t="n">
+        <v>0.9673611111111111</v>
+      </c>
+      <c r="D87" s="6" t="n">
+        <v>11.3</v>
+      </c>
+    </row>
     <row r="88">
-</row>
+      <c r="A88" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B88" s="4" t="n">
+        <v>0.002777777777777778</v>
+      </c>
+      <c r="D88" s="6" t="n">
+        <v>23.6</v>
+      </c>
+    </row>
     <row r="89">
-</row>
+      <c r="B89" s="12" t="n">
+        <v>0.015277777777777777</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="90">
-</row>
+      <c r="B90" s="4" t="n">
+        <v>0.017361111111111112</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="91">
-</row>
+      <c r="B91" s="4" t="n">
+        <v>0.020833333333333332</v>
+      </c>
+      <c r="E91" s="6" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
     <row r="92">
-</row>
+      <c r="B92" s="4" t="n">
+        <v>0.08611111111111111</v>
+      </c>
+      <c r="D92" s="6" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
     <row r="93">
-</row>
+      <c r="B93" s="4" t="n">
+        <v>0.1875</v>
+      </c>
+      <c r="D93" s="6" t="n">
+        <v>15.8</v>
+      </c>
+    </row>
     <row r="94">
-</row>
+      <c r="B94" s="4" t="n">
+        <v>0.2833333333333333</v>
+      </c>
+      <c r="D94" s="6" t="n">
+        <v>13.6</v>
+      </c>
+    </row>
     <row r="95">
-</row>
+      <c r="B95" s="4" t="n">
+        <v>0.36736111111111114</v>
+      </c>
+      <c r="D95" s="6" t="n">
+        <v>12.8</v>
+      </c>
+    </row>
     <row r="96">
-</row>
+      <c r="B96" s="4" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="97">
-</row>
+      <c r="B97" s="4" t="n">
+        <v>0.3819444444444444</v>
+      </c>
+      <c r="E97" s="6" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
     <row r="98">
-</row>
+      <c r="B98" s="4" t="n">
+        <v>0.46111111111111114</v>
+      </c>
+      <c r="D98" s="6" t="n">
+        <v>15.6</v>
+      </c>
+    </row>
     <row r="99">
-</row>
+      <c r="B99" s="4" t="n">
+        <v>0.5375</v>
+      </c>
+      <c r="D99" s="6" t="n">
+        <v>17.8</v>
+      </c>
+    </row>
     <row r="100">
-</row>
+      <c r="B100" s="4" t="n">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="D100" s="6" t="n">
+        <v>19.8</v>
+      </c>
+    </row>
     <row r="101">
-</row>
+      <c r="B101" s="4" t="n">
+        <v>0.6388888888888888</v>
+      </c>
+      <c r="D101" s="6" t="n">
+        <v>22.5</v>
+      </c>
+    </row>
     <row r="102">
-</row>
+      <c r="B102" s="4" t="n">
+        <v>0.6888888888888889</v>
+      </c>
+      <c r="D102" s="6" t="n">
+        <v>20.7</v>
+      </c>
+    </row>
     <row r="103">
-</row>
+      <c r="B103" s="4" t="n">
+        <v>0.6944444444444444</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="104">
-</row>
+      <c r="B104" s="4" t="n">
+        <v>0.7048611111111112</v>
+      </c>
+      <c r="E104" s="6" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
     <row r="105">
-</row>
+      <c r="B105" s="4" t="n">
+        <v>0.7805555555555556</v>
+      </c>
+      <c r="D105" s="6" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
     <row r="106">
-</row>
+      <c r="B106" s="4" t="n">
+        <v>0.8534722222222222</v>
+      </c>
+      <c r="D106" s="6" t="n">
+        <v>17.8</v>
+      </c>
+    </row>
     <row r="107">
-</row>
+      <c r="B107" s="4" t="n">
+        <v>0.9013888888888889</v>
+      </c>
+      <c r="D107" s="6" t="n">
+        <v>16.1</v>
+      </c>
+    </row>
     <row r="108">
-</row>
+      <c r="B108" s="4" t="n">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="D108" s="6" t="n">
+        <v>18.0</v>
+      </c>
+    </row>
     <row r="109">
 </row>
     <row r="110">
@@ -1172,6 +1332,8 @@
     <row r="199">
 </row>
     <row r="200">
+</row>
+    <row r="201">
 </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
enlarge the x label size.
</commit_message>
<xml_diff>
--- a/RawData/元宝血糖记录.xlsx
+++ b/RawData/元宝血糖记录.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>日期 dd-mm-yyyy</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>鸡胸35g</t>
+  </si>
+  <si>
+    <t>17-09-2020</t>
+  </si>
+  <si>
+    <t>鸡肉33g</t>
   </si>
 </sst>
 </file>
@@ -1150,23 +1156,80 @@
       </c>
     </row>
     <row r="109">
-</row>
+      <c r="B109" s="4" t="n">
+        <v>0.9958333333333333</v>
+      </c>
+      <c r="D109" s="6" t="n">
+        <v>20.7</v>
+      </c>
+    </row>
     <row r="110">
-</row>
+      <c r="A110" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B110" s="4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="111">
-</row>
+      <c r="B111" s="4" t="n">
+        <v>0.006944444444444444</v>
+      </c>
+      <c r="E111" s="6" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
     <row r="112">
-</row>
+      <c r="B112" s="4" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="D112" s="6" t="n">
+        <v>21.6</v>
+      </c>
+    </row>
     <row r="113">
-</row>
+      <c r="B113" s="4" t="n">
+        <v>0.1736111111111111</v>
+      </c>
+      <c r="D113" s="6" t="n">
+        <v>16.9</v>
+      </c>
+    </row>
     <row r="114">
-</row>
+      <c r="B114" s="4" t="n">
+        <v>0.2708333333333333</v>
+      </c>
+      <c r="D114" s="6" t="n">
+        <v>13.0</v>
+      </c>
+    </row>
     <row r="115">
-</row>
+      <c r="B115" s="4" t="n">
+        <v>0.3645833333333333</v>
+      </c>
+      <c r="D115" s="6" t="n">
+        <v>12.9</v>
+      </c>
+    </row>
     <row r="116">
-</row>
+      <c r="B116" s="4" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="117">
-</row>
+      <c r="B117" s="4" t="n">
+        <v>0.3819444444444444</v>
+      </c>
+      <c r="E117" s="6" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
     <row r="118">
 </row>
     <row r="119">

</xml_diff>